<commit_message>
Added sign text to the "Woods" region notes to help identify regions
</commit_message>
<xml_diff>
--- a/Spreadsheets/HabitatRegionInventory.xlsx
+++ b/Spreadsheets/HabitatRegionInventory.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stuart\Desktop\StuRegions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stuart\Documents\habiregions\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2387" uniqueCount="2339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="2356">
   <si>
     <t>Habitat Region Inventory</t>
   </si>
@@ -7056,6 +7056,397 @@
   </si>
   <si>
     <t>v1.0 - 02/10/2017 - Stuart</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Henry the avatar"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "But keeping their heads"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign: "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Divorcing them all"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Six wives he wed"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Rhondas"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sign: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"KEEP OFF"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "REST AREA"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Seat yourself. Waiter will serve you ."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "KEEP OFF"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sign: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"H A B I T A T" - Habitat Crossroads?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Ye Olde Bottle Shoppe"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "RHONDA'S Roadside Rhesort"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Tony's TEXAS STYLE BAR B Q"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "THE HERMITAGE"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "SOUVENIRS"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Native Art"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "THE HERMIT AGE"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7428,7 +7819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -10902,10 +11293,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C137"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10913,9 +11304,10 @@
     <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -10925,8 +11317,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2199</v>
       </c>
@@ -10934,7 +11329,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2200</v>
       </c>
@@ -10942,7 +11337,7 @@
         <v>2068</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2201</v>
       </c>
@@ -10950,7 +11345,7 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2202</v>
       </c>
@@ -10958,7 +11353,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2203</v>
       </c>
@@ -10966,7 +11361,7 @@
         <v>2071</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2204</v>
       </c>
@@ -10974,20 +11369,26 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2205</v>
       </c>
       <c r="C8" t="s">
         <v>2073</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2331</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2206</v>
       </c>
@@ -10995,7 +11396,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2207</v>
       </c>
@@ -11003,7 +11404,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2208</v>
       </c>
@@ -11011,23 +11412,29 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2209</v>
       </c>
       <c r="C13" t="s">
         <v>2077</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>2354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2210</v>
       </c>
       <c r="C14" t="s">
         <v>2078</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2211</v>
       </c>
@@ -11035,7 +11442,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2212</v>
       </c>
@@ -11043,7 +11450,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2213</v>
       </c>
@@ -11051,7 +11458,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2214</v>
       </c>
@@ -11059,7 +11466,7 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2215</v>
       </c>
@@ -11067,7 +11474,7 @@
         <v>2083</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2216</v>
       </c>
@@ -11075,7 +11482,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2217</v>
       </c>
@@ -11083,7 +11490,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2218</v>
       </c>
@@ -11091,7 +11498,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2219</v>
       </c>
@@ -11099,7 +11506,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2220</v>
       </c>
@@ -11107,7 +11514,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2221</v>
       </c>
@@ -11115,7 +11522,7 @@
         <v>2089</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2222</v>
       </c>
@@ -11123,7 +11530,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2223</v>
       </c>
@@ -11131,7 +11538,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2224</v>
       </c>
@@ -11139,15 +11546,18 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2225</v>
       </c>
       <c r="C29" t="s">
         <v>2093</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2226</v>
       </c>
@@ -11155,7 +11565,7 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2227</v>
       </c>
@@ -11163,7 +11573,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2228</v>
       </c>
@@ -11171,7 +11581,7 @@
         <v>2096</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2229</v>
       </c>
@@ -11179,15 +11589,18 @@
         <v>2097</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2230</v>
       </c>
       <c r="C34" t="s">
         <v>2098</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2231</v>
       </c>
@@ -11195,7 +11608,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2232</v>
       </c>
@@ -11203,7 +11616,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2233</v>
       </c>
@@ -11211,7 +11624,7 @@
         <v>2101</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2234</v>
       </c>
@@ -11219,7 +11632,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2235</v>
       </c>
@@ -11227,7 +11640,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2236</v>
       </c>
@@ -11235,7 +11648,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2237</v>
       </c>
@@ -11243,7 +11656,7 @@
         <v>2105</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2238</v>
       </c>
@@ -11251,7 +11664,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2239</v>
       </c>
@@ -11259,7 +11672,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2240</v>
       </c>
@@ -11267,7 +11680,7 @@
         <v>2108</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2241</v>
       </c>
@@ -11275,7 +11688,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2242</v>
       </c>
@@ -11283,7 +11696,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>2243</v>
       </c>
@@ -11291,7 +11704,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>2244</v>
       </c>
@@ -11299,15 +11712,18 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>2245</v>
       </c>
       <c r="C49" t="s">
         <v>2113</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>2246</v>
       </c>
@@ -11315,7 +11731,7 @@
         <v>2114</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>2247</v>
       </c>
@@ -11323,7 +11739,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>2248</v>
       </c>
@@ -11331,7 +11747,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>2249</v>
       </c>
@@ -11339,7 +11755,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>2250</v>
       </c>
@@ -11347,7 +11763,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>2251</v>
       </c>
@@ -11355,7 +11771,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>2252</v>
       </c>
@@ -11363,7 +11779,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>2253</v>
       </c>
@@ -11371,15 +11787,18 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>2254</v>
       </c>
       <c r="C58" t="s">
         <v>2122</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>2255</v>
       </c>
@@ -11387,7 +11806,7 @@
         <v>2123</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>2256</v>
       </c>
@@ -11395,7 +11814,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>2257</v>
       </c>
@@ -11403,7 +11822,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>2258</v>
       </c>
@@ -11411,7 +11830,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>2259</v>
       </c>
@@ -11419,7 +11838,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>2260</v>
       </c>
@@ -11427,47 +11846,62 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>2261</v>
       </c>
       <c r="C65" t="s">
         <v>2129</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>2262</v>
       </c>
       <c r="C66" t="s">
         <v>2130</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>2263</v>
       </c>
       <c r="C67" t="s">
         <v>2131</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>2264</v>
       </c>
       <c r="C68" t="s">
         <v>2132</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>2265</v>
       </c>
       <c r="C69" t="s">
         <v>2133</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>2266</v>
       </c>
@@ -11475,7 +11909,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>2267</v>
       </c>
@@ -11483,7 +11917,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>2268</v>
       </c>
@@ -11491,7 +11925,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>2269</v>
       </c>
@@ -11499,7 +11933,7 @@
         <v>2137</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>2270</v>
       </c>
@@ -11507,15 +11941,18 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>2271</v>
       </c>
       <c r="C75" t="s">
         <v>2139</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>2272</v>
       </c>
@@ -11523,7 +11960,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>2273</v>
       </c>
@@ -11531,7 +11968,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>2274</v>
       </c>
@@ -11539,7 +11976,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>2275</v>
       </c>
@@ -11547,7 +11984,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>2276</v>
       </c>
@@ -11555,7 +11992,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>2277</v>
       </c>
@@ -11563,15 +12000,18 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>2278</v>
       </c>
       <c r="C82" t="s">
         <v>2146</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>2279</v>
       </c>
@@ -11579,7 +12019,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>2280</v>
       </c>
@@ -11587,7 +12027,7 @@
         <v>2148</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>2281</v>
       </c>
@@ -11595,7 +12035,7 @@
         <v>2149</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>2282</v>
       </c>
@@ -11603,7 +12043,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>2283</v>
       </c>
@@ -11611,7 +12051,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>2284</v>
       </c>
@@ -11619,7 +12059,7 @@
         <v>2152</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>2285</v>
       </c>
@@ -11627,7 +12067,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>2286</v>
       </c>
@@ -11635,7 +12075,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>2287</v>
       </c>
@@ -11643,7 +12083,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>2288</v>
       </c>
@@ -11651,7 +12091,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>2289</v>
       </c>
@@ -11659,7 +12099,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>2290</v>
       </c>
@@ -11667,7 +12107,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>2291</v>
       </c>
@@ -11675,7 +12115,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>2292</v>
       </c>
@@ -11811,7 +12251,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>2309</v>
       </c>
@@ -11819,7 +12259,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>2310</v>
       </c>
@@ -11827,7 +12267,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>2311</v>
       </c>
@@ -11835,7 +12275,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>2312</v>
       </c>
@@ -11843,7 +12283,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>2313</v>
       </c>
@@ -11851,7 +12291,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>2314</v>
       </c>
@@ -11859,7 +12299,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>2315</v>
       </c>
@@ -11867,7 +12307,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>2316</v>
       </c>
@@ -11875,7 +12315,7 @@
         <v>2184</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>2317</v>
       </c>
@@ -11883,7 +12323,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>2318</v>
       </c>
@@ -11891,7 +12331,7 @@
         <v>2186</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>2319</v>
       </c>
@@ -11899,7 +12339,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>2320</v>
       </c>
@@ -11907,23 +12347,29 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>2321</v>
       </c>
       <c r="C125" t="s">
         <v>2189</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>2322</v>
       </c>
       <c r="C126" t="s">
         <v>2190</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>2323</v>
       </c>
@@ -11931,7 +12377,7 @@
         <v>2191</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>2324</v>
       </c>
@@ -12004,6 +12450,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>